<commit_message>
general and what's new page are finished
</commit_message>
<xml_diff>
--- a/src/test/test_data/magneto.xlsx
+++ b/src/test/test_data/magneto.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\magneto\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E0A001-9C0C-4A02-B907-A651ABEAA6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539A2FCB-DCC8-4ADC-9DF2-C7996A8AC3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Header" sheetId="2" r:id="rId2"/>
+    <sheet name="women" sheetId="2" r:id="rId2"/>
     <sheet name="UserManagement" sheetId="3" r:id="rId3"/>
     <sheet name="ChecklistManagement" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="157">
   <si>
     <t>tc_id</t>
   </si>
@@ -96,21 +96,9 @@
     <t>menuItems1</t>
   </si>
   <si>
-    <t>menuItems0</t>
-  </si>
-  <si>
-    <t>menuItems2</t>
-  </si>
-  <si>
-    <t>LICENCE OVERVIEW</t>
-  </si>
-  <si>
     <t>USER MANAGEMENT</t>
   </si>
   <si>
-    <t>CHECKLIST MANAGEMENT</t>
-  </si>
-  <si>
     <t>loginText</t>
   </si>
   <si>
@@ -123,12 +111,6 @@
     <t>Your information was successfully saved</t>
   </si>
   <si>
-    <t>firstnameAS</t>
-  </si>
-  <si>
-    <t>lastnameAS</t>
-  </si>
-  <si>
     <t>accountFirstEmptyMessage</t>
   </si>
   <si>
@@ -162,12 +144,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>sasa_NOTrandom</t>
-  </si>
-  <si>
-    <t>stjepanovic_NOTrandom</t>
-  </si>
-  <si>
     <t>firstNameTechnician</t>
   </si>
   <si>
@@ -349,6 +325,183 @@
   </si>
   <si>
     <t>Thank you for registering with Fake Online Clothing Store.</t>
+  </si>
+  <si>
+    <t>invalidMessageCreateAccount</t>
+  </si>
+  <si>
+    <t>This is a required field.</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>SI_009</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>stjepanovic1</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address (Ex: johndoe@domain.com).</t>
+  </si>
+  <si>
+    <t>SI_010</t>
+  </si>
+  <si>
+    <t>SI_011</t>
+  </si>
+  <si>
+    <t>SI_012</t>
+  </si>
+  <si>
+    <t>SI_013</t>
+  </si>
+  <si>
+    <t>SI_014</t>
+  </si>
+  <si>
+    <t>SI_015</t>
+  </si>
+  <si>
+    <t>stjepa</t>
+  </si>
+  <si>
+    <t>Password Strength: No Password</t>
+  </si>
+  <si>
+    <t>Password Strength: Weak</t>
+  </si>
+  <si>
+    <t>Password Strength: Very Strong</t>
+  </si>
+  <si>
+    <t>strengthpassword</t>
+  </si>
+  <si>
+    <t>Kikinda1</t>
+  </si>
+  <si>
+    <t>Password Strength: Medium</t>
+  </si>
+  <si>
+    <t>Stjepanovic</t>
+  </si>
+  <si>
+    <t>Please enter the same value again.</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>The account sign-in was incorrect or your account is disabled temporarily. Please wait and try again later.</t>
+  </si>
+  <si>
+    <t>invalidMessageCreateAccount2</t>
+  </si>
+  <si>
+    <t>Incorrect CAPTCHA</t>
+  </si>
+  <si>
+    <t>emptyCartMessage</t>
+  </si>
+  <si>
+    <t>You have no items in your shopping cart.</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>What's New</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>menuItemTitle1</t>
+  </si>
+  <si>
+    <t>menuItemTitle3</t>
+  </si>
+  <si>
+    <t>menuItemTitle2</t>
+  </si>
+  <si>
+    <t>TOPS</t>
+  </si>
+  <si>
+    <t>BOTTOMS</t>
+  </si>
+  <si>
+    <t>NEW IN WOMEN'S</t>
+  </si>
+  <si>
+    <t>NEW IN MEN'S</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>Hoodies &amp; Sweatshirts</t>
+  </si>
+  <si>
+    <t>Jackets</t>
+  </si>
+  <si>
+    <t>Tees</t>
+  </si>
+  <si>
+    <t>Bras &amp; Tanks</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Shorts</t>
+  </si>
+  <si>
+    <t>menuItemTitle2Sub</t>
+  </si>
+  <si>
+    <t>firstPageYesNo</t>
+  </si>
+  <si>
+    <t>productType</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>Tanks</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>hoverItem</t>
   </si>
 </sst>
 </file>
@@ -470,7 +623,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -522,11 +675,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -547,9 +713,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -568,6 +731,25 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,10 +763,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -604,14 +786,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,7 +1092,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,205 +1114,855 @@
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="20.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="37.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-    </row>
-    <row r="2" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+    </row>
+    <row r="2" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+    </row>
+    <row r="3" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="B4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="17"/>
+      <c r="M4" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="30" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="U6" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="S8" s="21"/>
+      <c r="T8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="U8" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
+      <c r="B9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="S9" s="17"/>
+      <c r="T9" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="S10" s="7"/>
+      <c r="T10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U11" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="U12" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V12" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="U14" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V14" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U15" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V15" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="U16" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="V16" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1148,279 +1972,761 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16" width="21" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="21" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="1" customWidth="1"/>
     <col min="17" max="17" width="24" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="20" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-    </row>
-    <row r="2" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+    </row>
+    <row r="2" spans="1:22" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+    </row>
+    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="11" t="s">
+      <c r="H3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="V4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="U6" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="7"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="V7" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="S8" s="21"/>
+      <c r="T8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="U8" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="S9" s="17"/>
+      <c r="T9" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="S10" s="7"/>
+      <c r="T10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U11" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="U12" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V12" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V13" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="U14" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V14" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U15" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V15" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="U16" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="V16" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1454,116 +2760,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
     </row>
     <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z3" s="13" t="s">
+      <c r="W3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1584,23 +2890,23 @@
         <v>13</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
@@ -1609,20 +2915,20 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="T4" s="9"/>
       <c r="U4" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y4" s="9"/>
       <c r="Z4" s="5" t="s">
@@ -1647,17 +2953,17 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -1669,22 +2975,22 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z5" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1704,23 +3010,23 @@
         <v>13</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -1731,16 +3037,16 @@
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
       <c r="U6" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y6" s="9"/>
       <c r="Z6" s="5" t="s">
@@ -1764,34 +3070,34 @@
         <v>13</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="N7" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
@@ -1799,16 +3105,16 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X7" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y7" s="9"/>
       <c r="Z7" s="5" t="s">
@@ -1832,53 +3138,53 @@
         <v>13</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y8" s="9"/>
       <c r="Z8" s="5" t="s">
@@ -1902,53 +3208,53 @@
         <v>13</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X9" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y9" s="9"/>
       <c r="Z9" s="5" t="s">
@@ -1957,7 +3263,7 @@
     </row>
     <row r="10" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
@@ -1972,57 +3278,57 @@
         <v>13</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="N10" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="S10" s="8"/>
       <c r="T10" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y10" s="9"/>
       <c r="Z10" s="5" t="s">
@@ -2031,7 +3337,7 @@
     </row>
     <row r="11" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -2046,55 +3352,55 @@
         <v>13</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Y11" s="9"/>
       <c r="Z11" s="5" t="s">
@@ -2148,120 +3454,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
     </row>
     <row r="2" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="15" t="s">
+      <c r="H3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="R3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" s="15" t="s">
+      <c r="X3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2282,56 +3588,56 @@
         <v>13</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
       <c r="V4" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z4" s="9"/>
       <c r="AA4" s="5" t="s">
@@ -2355,60 +3661,60 @@
         <v>13</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,54 +3734,54 @@
         <v>13</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y6" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z6" s="9"/>
       <c r="AA6" s="5" t="s">
@@ -2500,55 +3806,55 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
       <c r="V7" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X7" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y7" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z7" s="9"/>
       <c r="AA7" s="5" t="s">
@@ -2573,57 +3879,57 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X8" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y8" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z8" s="9"/>
       <c r="AA8" s="5" t="s">
@@ -2641,62 +3947,62 @@
         <v>8</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X9" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y9" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z9" s="9"/>
       <c r="AA9" s="5" t="s">
@@ -2705,7 +4011,7 @@
     </row>
     <row r="10" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
@@ -2721,13 +4027,13 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -2741,19 +4047,19 @@
       <c r="S10" s="9"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z10" s="9"/>
       <c r="AA10" s="5" t="s">
@@ -2762,7 +4068,7 @@
     </row>
     <row r="11" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -2778,13 +4084,13 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -2798,19 +4104,19 @@
       <c r="S11" s="9"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Y11" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z11" s="9"/>
       <c r="AA11" s="5" t="s">

</xml_diff>

<commit_message>
choosing menu items over hover option
</commit_message>
<xml_diff>
--- a/src/test/test_data/magneto.xlsx
+++ b/src/test/test_data/magneto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\magneto\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539A2FCB-DCC8-4ADC-9DF2-C7996A8AC3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3350F0CC-D5B7-4F1E-9EF3-E3890504E99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="167">
   <si>
     <t>tc_id</t>
   </si>
@@ -502,6 +502,36 @@
   </si>
   <si>
     <t>hoverItem</t>
+  </si>
+  <si>
+    <t>hoverSubItem</t>
+  </si>
+  <si>
+    <t>Tops</t>
+  </si>
+  <si>
+    <t>Bottoms</t>
+  </si>
+  <si>
+    <t>Bags</t>
+  </si>
+  <si>
+    <t>Fitness Equipment</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>hoverSubSubItem</t>
+  </si>
+  <si>
+    <t>Video Download</t>
+  </si>
+  <si>
+    <t>SI_016</t>
+  </si>
+  <si>
+    <t>SI_017</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P9"/>
+    <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,17 +2024,19 @@
     <col min="13" max="13" width="17.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21" style="1" customWidth="1"/>
-    <col min="17" max="17" width="24" style="1" customWidth="1"/>
-    <col min="18" max="18" width="20" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="17" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="14.42578125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -2029,12 +2061,14 @@
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
       <c r="V1" s="30"/>
-    </row>
-    <row r="2" spans="1:22" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+    </row>
+    <row r="2" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="26"/>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -2080,29 +2114,35 @@
       <c r="O3" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="R3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="W3" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="X3" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2133,28 +2173,34 @@
         <v>131</v>
       </c>
       <c r="P4" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="R4" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="S4" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="T4" s="17" t="s">
         <v>143</v>
       </c>
       <c r="U4" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="W4" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="X4" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2181,32 +2227,38 @@
       <c r="N5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="R5" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="S5" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="S5" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="T5" s="17" t="s">
         <v>143</v>
       </c>
       <c r="U5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="W5" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V5" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2229,32 +2281,38 @@
       <c r="N6" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="P6" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="R6" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="S6" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="T6" s="17" t="s">
         <v>144</v>
       </c>
       <c r="U6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="W6" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V6" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X6" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2278,27 +2336,33 @@
         <v>102</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="P7" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="Q7" s="17"/>
+      <c r="P7" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>146</v>
+      </c>
       <c r="R7" s="17" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="S7" s="17"/>
       <c r="T7" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="U7" s="17" t="s">
+      <c r="U7" s="17"/>
+      <c r="V7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="W7" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V7" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X7" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -2321,28 +2385,34 @@
       <c r="N8" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="O8" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="P8" s="17" t="s">
+      <c r="O8" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="Q8" s="21"/>
+      <c r="P8" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="R8" s="17" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="S8" s="21"/>
       <c r="T8" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="U8" s="17" t="s">
+      <c r="U8" s="21"/>
+      <c r="V8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="W8" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="V8" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X8" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2365,26 +2435,34 @@
       <c r="N9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17" t="s">
+      <c r="O9" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="21" t="s">
-        <v>147</v>
+      <c r="P9" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="R9" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="S9" s="17"/>
       <c r="T9" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="U9" s="17" t="s">
+      <c r="U9" s="17"/>
+      <c r="V9" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="W9" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="V9" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -2407,26 +2485,34 @@
       <c r="N10" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="R10" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="U10" s="17" t="s">
+      <c r="U10" s="7"/>
+      <c r="V10" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="W10" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="V10" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="X10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
@@ -2453,22 +2539,30 @@
       <c r="N11" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="O11" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>161</v>
+      </c>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
-      <c r="T11" s="17" t="s">
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="U11" s="17" t="s">
+      <c r="W11" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V11" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="X11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
@@ -2491,22 +2585,30 @@
       <c r="N12" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="O12" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
-      <c r="T12" s="17" t="s">
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="U12" s="17" t="s">
+      <c r="W12" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V12" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X12" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>107</v>
       </c>
@@ -2529,22 +2631,30 @@
       <c r="N13" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+      <c r="O13" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>164</v>
+      </c>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
-      <c r="T13" s="17" t="s">
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="U13" s="17" t="s">
+      <c r="W13" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V13" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X13" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>108</v>
       </c>
@@ -2567,22 +2677,30 @@
       <c r="N14" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
+      <c r="O14" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
-      <c r="T14" s="17" t="s">
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="U14" s="17" t="s">
+      <c r="W14" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V14" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="X14" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
@@ -2605,22 +2723,30 @@
       <c r="N15" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
+      <c r="O15" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
-      <c r="T15" s="21" t="s">
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="U15" s="17" t="s">
+      <c r="W15" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V15" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="X15" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>110</v>
       </c>
@@ -2643,22 +2769,30 @@
       <c r="N16" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
+      <c r="O16" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>162</v>
+      </c>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
-      <c r="T16" s="17" t="s">
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="U16" s="17" t="s">
+      <c r="W16" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="V16" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="X16" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>111</v>
       </c>
@@ -2687,16 +2821,26 @@
       <c r="N17" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
+      <c r="O17" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>153</v>
+      </c>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W17" s="7"/>
+      <c r="X17" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>112</v>
       </c>
@@ -2713,20 +2857,134 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+      <c r="O18" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="P18" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>148</v>
+      </c>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
+      <c r="X18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y18" s="7"/>
+    </row>
+    <row r="19" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q19" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="R19" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="S19" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="T19" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U19" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="V19" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="W19" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="X19" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="W20" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="X20" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
women page is finshed
</commit_message>
<xml_diff>
--- a/src/test/test_data/magneto.xlsx
+++ b/src/test/test_data/magneto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QA projekti\Automation_projekti\magneto\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6E5404-FEDA-41D3-956D-50C3ACCC5064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCD263-9577-4523-9BE2-C182B2D1E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="181">
   <si>
     <t>tc_id</t>
   </si>
@@ -564,10 +564,16 @@
     <t>Erin Recommends</t>
   </si>
   <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Solid</t>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -816,6 +822,7 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,7 +859,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,35 +1207,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
     </row>
     <row r="2" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2041,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD393A5-6731-4B8E-BE1C-8BAF208C9B9B}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,7 +2073,7 @@
     <col min="19" max="19" width="24" style="1" customWidth="1"/>
     <col min="20" max="20" width="20" style="1" customWidth="1"/>
     <col min="21" max="22" width="17.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="19.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="21.5703125" style="1" customWidth="1"/>
     <col min="24" max="24" width="17" style="1" customWidth="1"/>
     <col min="25" max="25" width="15.7109375" style="1" customWidth="1"/>
     <col min="26" max="26" width="14.42578125" style="1" customWidth="1"/>
@@ -2075,38 +2081,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
     </row>
     <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -2360,11 +2366,11 @@
       <c r="U6" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="V6" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="W6" s="17" t="s">
-        <v>178</v>
+      <c r="V6" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="W6" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="X6" s="17" t="s">
         <v>144</v>
@@ -2473,10 +2479,10 @@
       </c>
       <c r="U8" s="21"/>
       <c r="V8" s="21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="W8" s="21" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="X8" s="17" t="s">
         <v>146</v>
@@ -2528,8 +2534,12 @@
         <v>147</v>
       </c>
       <c r="U9" s="17"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
+      <c r="V9" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="W9" s="21" t="s">
+        <v>180</v>
+      </c>
       <c r="X9" s="21" t="s">
         <v>147</v>
       </c>
@@ -2824,8 +2834,8 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
       <c r="X15" s="21" t="s">
         <v>147</v>
       </c>
@@ -3069,8 +3079,8 @@
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
       <c r="X20" s="21" t="s">
         <v>147</v>
       </c>
@@ -3118,38 +3128,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -3812,39 +3822,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
     </row>
     <row r="2" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
     </row>
     <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">

</xml_diff>